<commit_message>
u matrix: electricity use from gas boiler put to zero
</commit_message>
<xml_diff>
--- a/User A/inputs/u - Support.xlsx
+++ b/User A/inputs/u - Support.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\eNextHub\MARIOU-RESBEV\User A\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A23B2B9-511B-8646-B22A-9D465C9BBA59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0DABC3E-D6B0-44A4-A29C-79E269485A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="2000" windowWidth="26300" windowHeight="15440" xr2:uid="{40DF600A-E5F2-F843-969F-9E4CA1CA9BEB}"/>
+    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15720" xr2:uid="{40DF600A-E5F2-F843-969F-9E4CA1CA9BEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -570,37 +570,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5233747B-244C-394F-9967-C406E805DD5B}">
   <dimension ref="A1:V10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="34.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30.625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -666,7 +666,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
         <v>21</v>
@@ -732,7 +732,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
@@ -760,7 +760,7 @@
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
@@ -783,7 +783,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="1">
         <v>0.25</v>
@@ -792,7 +792,7 @@
         <v>0.15</v>
       </c>
       <c r="K4" s="1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="L4" s="1">
         <v>0</v>
@@ -807,7 +807,7 @@
         <v>0</v>
       </c>
       <c r="P4" s="1">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="1">
         <v>1.05</v>
@@ -828,7 +828,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>28</v>
       </c>
@@ -896,7 +896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>29</v>
       </c>
@@ -964,7 +964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>30</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>31</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>32</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>33</v>
       </c>

</xml_diff>